<commit_message>
Update values and reports
</commit_message>
<xml_diff>
--- a/weekly/2025-CW12_weight_tracking.xlsx
+++ b/weekly/2025-CW12_weight_tracking.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,14 +486,138 @@
       <c r="B2" t="n">
         <v>95.59999999999999</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>96.09999999999999</v>
+      </c>
       <c r="D2" t="n">
         <v>28.4</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>27.5</v>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="B3" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>94.8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28.6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45963</v>
+      </c>
+      <c r="B4" t="n">
+        <v>94.7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="D4" t="n">
+        <v>28</v>
+      </c>
+      <c r="E4" t="n">
+        <v>28</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45964</v>
+      </c>
+      <c r="B5" t="n">
+        <v>95</v>
+      </c>
+      <c r="C5" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="E5" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B6" t="n">
+        <v>94.90000000000001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="D6" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45966</v>
+      </c>
+      <c r="B7" t="n">
+        <v>94.40000000000001</v>
+      </c>
+      <c r="C7" t="n">
+        <v>95</v>
+      </c>
+      <c r="D7" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45967</v>
+      </c>
+      <c r="B8" t="n">
+        <v>94.3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>94.90000000000001</v>
+      </c>
+      <c r="D8" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>